<commit_message>
seed lot has seed weith instead of number of seed
</commit_message>
<xml_diff>
--- a/vavilov_pedigree/test/data/seed_lots.xlsx
+++ b/vavilov_pedigree/test/data/seed_lots.xlsx
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Description</t>
   </si>
   <si>
-    <t xml:space="preserve">NumSeeds</t>
+    <t xml:space="preserve">SeedsWeight</t>
   </si>
   <si>
     <t xml:space="preserve">selot1</t>
@@ -184,8 +184,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -209,148 +213,151 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="1" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <v>454</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <v>23</v>
       </c>
     </row>

</xml_diff>